<commit_message>
work in progress for final
</commit_message>
<xml_diff>
--- a/CargoUIAutomation/src/test/resources/XpathTestData.xlsx
+++ b/CargoUIAutomation/src/test/resources/XpathTestData.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalFiles\p57448\CargoUIAutomation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\IdeaProjects\Cargo\CargoUIAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2C7D7B-8119-4E62-9390-7002EBD9A625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE42381-7505-45E5-8C73-85A66FEA8288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{73F83708-58D9-CD41-B3DD-01428282C24F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73F83708-58D9-CD41-B3DD-01428282C24F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="306">
   <si>
     <t>CargoUsernameLogin</t>
   </si>
@@ -659,30 +648,6 @@
     <t>gbParcelsDepartureTime</t>
   </si>
   <si>
-    <t>gbParcelsShipmentServiceDoortoDoor</t>
-  </si>
-  <si>
-    <t>label[for='generalSelectedPickupDeliveryOptionCode0']</t>
-  </si>
-  <si>
-    <t>gbParcelsShipmentServicePickuponly</t>
-  </si>
-  <si>
-    <t>label[for='generalSelectedPickupDeliveryOptionCode1']</t>
-  </si>
-  <si>
-    <t>gbParcelsShipmentServiceDeliveryOnly</t>
-  </si>
-  <si>
-    <t>label[for='generalSelectedPickupDeliveryOptionCode2']</t>
-  </si>
-  <si>
-    <t>gbParcelsShipmentServiceNone</t>
-  </si>
-  <si>
-    <t>label[for='generalSelectedPickupDeliveryOptionCode3']</t>
-  </si>
-  <si>
     <t>gbParcels1stParcel</t>
   </si>
   <si>
@@ -972,6 +937,12 @@
   </si>
   <si>
     <t>#boaccountNbr-1</t>
+  </si>
+  <si>
+    <t>gbParcelsShipmentServiceDeliveryType</t>
+  </si>
+  <si>
+    <t>input[id*='generalSelectedPickupDeliveryOptionCode'] + label[for='%s']</t>
   </si>
 </sst>
 </file>
@@ -1365,21 +1336,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486E0D93-E580-4D4E-91BE-77049C6FF4F1}">
-  <dimension ref="A1:C163"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A134" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="56.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.296875" style="1" customWidth="1"/>
     <col min="3" max="3" width="73.5" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5">
+    <row r="1" spans="1:3" ht="16.8">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1387,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5">
+    <row r="2" spans="1:3" ht="16.8">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5">
+    <row r="3" spans="1:3" ht="16.8">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5">
+    <row r="4" spans="1:3" ht="16.8">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5">
+    <row r="5" spans="1:3" ht="16.8">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1419,7 +1390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5">
+    <row r="6" spans="1:3" ht="16.8">
       <c r="A6" s="2" t="s">
         <v>170</v>
       </c>
@@ -1427,7 +1398,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5">
+    <row r="7" spans="1:3" ht="16.8">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
@@ -1435,7 +1406,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5">
+    <row r="8" spans="1:3" ht="16.8">
       <c r="A8" s="2" t="s">
         <v>174</v>
       </c>
@@ -1443,7 +1414,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5">
+    <row r="9" spans="1:3" ht="16.8">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1451,7 +1422,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5">
+    <row r="10" spans="1:3" ht="16.8">
       <c r="A10" s="2" t="s">
         <v>179</v>
       </c>
@@ -1462,7 +1433,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5">
+    <row r="11" spans="1:3" ht="16.8">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1471,7 +1442,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="16.5">
+    <row r="12" spans="1:3" ht="16.8">
       <c r="A12" s="2" t="s">
         <v>180</v>
       </c>
@@ -1480,7 +1451,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="16.5">
+    <row r="13" spans="1:3" ht="16.8">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1488,7 +1459,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5">
+    <row r="14" spans="1:3" ht="16.8">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1496,7 +1467,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5">
+    <row r="15" spans="1:3" ht="16.8">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1504,7 +1475,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5">
+    <row r="16" spans="1:3" ht="16.8">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1512,7 +1483,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.5">
+    <row r="17" spans="1:2" ht="16.8">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1520,7 +1491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.5">
+    <row r="18" spans="1:2" ht="16.8">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1528,7 +1499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.5">
+    <row r="19" spans="1:2" ht="16.8">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1536,7 +1507,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.5">
+    <row r="20" spans="1:2" ht="16.8">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1544,7 +1515,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16.5">
+    <row r="21" spans="1:2" ht="16.8">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1552,7 +1523,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.5">
+    <row r="22" spans="1:2" ht="16.8">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1560,7 +1531,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.5">
+    <row r="23" spans="1:2" ht="16.8">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1568,7 +1539,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.5">
+    <row r="24" spans="1:2" ht="16.8">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -1576,7 +1547,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.5">
+    <row r="25" spans="1:2" ht="16.8">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1584,7 +1555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.5">
+    <row r="26" spans="1:2" ht="16.8">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -1592,7 +1563,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.5">
+    <row r="27" spans="1:2" ht="16.8">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1600,7 +1571,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.5">
+    <row r="28" spans="1:2" ht="16.8">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1608,7 +1579,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16.5">
+    <row r="29" spans="1:2" ht="16.8">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -1616,7 +1587,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.5">
+    <row r="30" spans="1:2" ht="16.8">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1624,7 +1595,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.5">
+    <row r="31" spans="1:2" ht="16.8">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -1632,7 +1603,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16.5">
+    <row r="32" spans="1:2" ht="16.8">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -1640,7 +1611,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16.5">
+    <row r="33" spans="1:2" ht="16.8">
       <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
@@ -1648,7 +1619,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16.5">
+    <row r="34" spans="1:2" ht="16.8">
       <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
@@ -1656,7 +1627,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16.5">
+    <row r="35" spans="1:2" ht="16.8">
       <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
@@ -1664,7 +1635,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16.5">
+    <row r="36" spans="1:2" ht="16.8">
       <c r="A36" s="2" t="s">
         <v>54</v>
       </c>
@@ -1672,7 +1643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16.5">
+    <row r="37" spans="1:2" ht="16.8">
       <c r="A37" s="2" t="s">
         <v>56</v>
       </c>
@@ -1680,7 +1651,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.5">
+    <row r="38" spans="1:2" ht="16.8">
       <c r="A38" s="2" t="s">
         <v>58</v>
       </c>
@@ -1688,7 +1659,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.5">
+    <row r="39" spans="1:2" ht="16.8">
       <c r="A39" s="2" t="s">
         <v>60</v>
       </c>
@@ -1696,7 +1667,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.5">
+    <row r="40" spans="1:2" ht="16.8">
       <c r="A40" s="2" t="s">
         <v>62</v>
       </c>
@@ -1704,7 +1675,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16.5">
+    <row r="41" spans="1:2" ht="16.8">
       <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
@@ -1712,7 +1683,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16.5">
+    <row r="42" spans="1:2" ht="16.8">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -1720,7 +1691,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.5">
+    <row r="43" spans="1:2" ht="16.8">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -1728,7 +1699,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16.5">
+    <row r="44" spans="1:2" ht="16.8">
       <c r="A44" s="2" t="s">
         <v>70</v>
       </c>
@@ -1736,7 +1707,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="16.5">
+    <row r="45" spans="1:2" ht="16.8">
       <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
@@ -1744,7 +1715,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16.5">
+    <row r="46" spans="1:2" ht="16.8">
       <c r="A46" s="2" t="s">
         <v>74</v>
       </c>
@@ -1752,7 +1723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16.5">
+    <row r="47" spans="1:2" ht="16.8">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
@@ -1760,7 +1731,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16.5">
+    <row r="48" spans="1:2" ht="16.8">
       <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
@@ -1768,7 +1739,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16.5">
+    <row r="49" spans="1:2" ht="16.8">
       <c r="A49" s="2" t="s">
         <v>80</v>
       </c>
@@ -1776,7 +1747,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16.5">
+    <row r="50" spans="1:2" ht="16.8">
       <c r="A50" s="2" t="s">
         <v>82</v>
       </c>
@@ -1784,7 +1755,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16.5">
+    <row r="51" spans="1:2" ht="16.8">
       <c r="A51" s="2" t="s">
         <v>84</v>
       </c>
@@ -1792,7 +1763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16.5">
+    <row r="52" spans="1:2" ht="16.8">
       <c r="A52" s="2" t="s">
         <v>86</v>
       </c>
@@ -1800,7 +1771,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16.5">
+    <row r="53" spans="1:2" ht="16.8">
       <c r="A53" s="2" t="s">
         <v>88</v>
       </c>
@@ -1808,7 +1779,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16.5">
+    <row r="54" spans="1:2" ht="16.8">
       <c r="A54" s="2" t="s">
         <v>90</v>
       </c>
@@ -1816,7 +1787,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16.5">
+    <row r="55" spans="1:2" ht="16.8">
       <c r="A55" s="2" t="s">
         <v>92</v>
       </c>
@@ -1824,7 +1795,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16.5">
+    <row r="56" spans="1:2" ht="16.8">
       <c r="A56" s="2" t="s">
         <v>94</v>
       </c>
@@ -1832,7 +1803,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16.5">
+    <row r="57" spans="1:2" ht="16.8">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -1840,7 +1811,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16.5">
+    <row r="58" spans="1:2" ht="16.8">
       <c r="A58" s="2" t="s">
         <v>98</v>
       </c>
@@ -1848,7 +1819,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16.5">
+    <row r="59" spans="1:2" ht="16.8">
       <c r="A59" s="2" t="s">
         <v>100</v>
       </c>
@@ -1856,7 +1827,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16.5">
+    <row r="60" spans="1:2" ht="16.8">
       <c r="A60" s="2" t="s">
         <v>102</v>
       </c>
@@ -1864,7 +1835,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16.5">
+    <row r="61" spans="1:2" ht="16.8">
       <c r="A61" s="2" t="s">
         <v>104</v>
       </c>
@@ -1872,7 +1843,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16.5">
+    <row r="62" spans="1:2" ht="16.8">
       <c r="A62" s="2" t="s">
         <v>106</v>
       </c>
@@ -1880,7 +1851,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.5">
+    <row r="63" spans="1:2" ht="16.8">
       <c r="A63" s="2" t="s">
         <v>108</v>
       </c>
@@ -1888,7 +1859,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16.5">
+    <row r="64" spans="1:2" ht="16.8">
       <c r="A64" s="2" t="s">
         <v>110</v>
       </c>
@@ -1896,7 +1867,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="16.5">
+    <row r="65" spans="1:2" ht="16.8">
       <c r="A65" s="2" t="s">
         <v>112</v>
       </c>
@@ -1904,7 +1875,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16.5">
+    <row r="66" spans="1:2" ht="16.8">
       <c r="A66" s="2" t="s">
         <v>114</v>
       </c>
@@ -1912,7 +1883,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16.5">
+    <row r="67" spans="1:2" ht="16.8">
       <c r="A67" s="2" t="s">
         <v>116</v>
       </c>
@@ -1920,7 +1891,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="16.5">
+    <row r="68" spans="1:2" ht="16.8">
       <c r="A68" s="2" t="s">
         <v>118</v>
       </c>
@@ -1928,7 +1899,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16.5">
+    <row r="69" spans="1:2" ht="16.8">
       <c r="A69" s="2" t="s">
         <v>120</v>
       </c>
@@ -1936,7 +1907,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="16.5">
+    <row r="70" spans="1:2" ht="16.8">
       <c r="A70" s="2" t="s">
         <v>122</v>
       </c>
@@ -1944,7 +1915,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="16.5">
+    <row r="71" spans="1:2" ht="16.8">
       <c r="A71" s="2" t="s">
         <v>124</v>
       </c>
@@ -1952,7 +1923,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16.5">
+    <row r="72" spans="1:2" ht="16.8">
       <c r="A72" s="2" t="s">
         <v>126</v>
       </c>
@@ -1960,7 +1931,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16.5">
+    <row r="73" spans="1:2" ht="16.8">
       <c r="A73" s="2" t="s">
         <v>128</v>
       </c>
@@ -1968,7 +1939,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="16.5">
+    <row r="74" spans="1:2" ht="16.8">
       <c r="A74" s="2" t="s">
         <v>129</v>
       </c>
@@ -1976,7 +1947,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="16.5">
+    <row r="75" spans="1:2" ht="16.8">
       <c r="A75" s="2" t="s">
         <v>131</v>
       </c>
@@ -1984,7 +1955,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="16.5">
+    <row r="76" spans="1:2" ht="16.8">
       <c r="A76" s="2" t="s">
         <v>133</v>
       </c>
@@ -1992,7 +1963,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="16.5">
+    <row r="77" spans="1:2" ht="16.8">
       <c r="A77" s="2" t="s">
         <v>135</v>
       </c>
@@ -2000,7 +1971,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="16.5">
+    <row r="78" spans="1:2" ht="16.8">
       <c r="A78" s="2" t="s">
         <v>137</v>
       </c>
@@ -2008,7 +1979,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16.5">
+    <row r="79" spans="1:2" ht="16.8">
       <c r="A79" s="2" t="s">
         <v>139</v>
       </c>
@@ -2016,7 +1987,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="16.5">
+    <row r="80" spans="1:2" ht="16.8">
       <c r="A80" s="2" t="s">
         <v>141</v>
       </c>
@@ -2024,7 +1995,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="16.5">
+    <row r="81" spans="1:2" ht="16.8">
       <c r="A81" s="2" t="s">
         <v>142</v>
       </c>
@@ -2032,7 +2003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16.5">
+    <row r="82" spans="1:2" ht="16.8">
       <c r="A82" s="2" t="s">
         <v>143</v>
       </c>
@@ -2040,7 +2011,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16.5">
+    <row r="83" spans="1:2" ht="16.8">
       <c r="A83" s="2" t="s">
         <v>145</v>
       </c>
@@ -2048,7 +2019,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16.5">
+    <row r="84" spans="1:2" ht="16.8">
       <c r="A84" s="2" t="s">
         <v>147</v>
       </c>
@@ -2056,7 +2027,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16.5">
+    <row r="85" spans="1:2" ht="16.8">
       <c r="A85" s="2" t="s">
         <v>149</v>
       </c>
@@ -2064,7 +2035,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16.5">
+    <row r="86" spans="1:2" ht="16.8">
       <c r="A86" s="2" t="s">
         <v>151</v>
       </c>
@@ -2072,7 +2043,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16.5">
+    <row r="87" spans="1:2" ht="16.8">
       <c r="A87" s="2" t="s">
         <v>153</v>
       </c>
@@ -2080,7 +2051,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16.5">
+    <row r="88" spans="1:2" ht="16.8">
       <c r="A88" s="2" t="s">
         <v>155</v>
       </c>
@@ -2088,7 +2059,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16.5">
+    <row r="89" spans="1:2" ht="16.8">
       <c r="A89" s="2" t="s">
         <v>157</v>
       </c>
@@ -2096,7 +2067,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="16.5">
+    <row r="90" spans="1:2" ht="16.8">
       <c r="A90" s="2" t="s">
         <v>159</v>
       </c>
@@ -2104,7 +2075,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16.5">
+    <row r="91" spans="1:2" ht="16.8">
       <c r="A91" s="2" t="s">
         <v>160</v>
       </c>
@@ -2112,7 +2083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16.5">
+    <row r="92" spans="1:2" ht="16.8">
       <c r="A92" s="2" t="s">
         <v>161</v>
       </c>
@@ -2120,7 +2091,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="16.5">
+    <row r="93" spans="1:2" ht="16.8">
       <c r="A93" s="2" t="s">
         <v>162</v>
       </c>
@@ -2128,7 +2099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="16.5">
+    <row r="94" spans="1:2" ht="16.8">
       <c r="A94" s="2" t="s">
         <v>163</v>
       </c>
@@ -2136,7 +2107,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="16.5">
+    <row r="95" spans="1:2" ht="16.8">
       <c r="A95" s="2" t="s">
         <v>165</v>
       </c>
@@ -2144,7 +2115,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="16.5">
+    <row r="96" spans="1:2" ht="16.8">
       <c r="A96" s="2" t="s">
         <v>167</v>
       </c>
@@ -2229,7 +2200,7 @@
         <v>203</v>
       </c>
       <c r="B106" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2237,55 +2208,55 @@
         <v>204</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2293,7 +2264,7 @@
         <v>205</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2301,377 +2272,353 @@
         <v>206</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1" t="s">
-        <v>207</v>
+        <v>304</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>208</v>
+        <v>305</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>256</v>
+        <v>303</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>53</v>
+        <v>288</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed Test Class Pharma
</commit_message>
<xml_diff>
--- a/CargoUIAutomation/src/test/resources/XpathTestData.xlsx
+++ b/CargoUIAutomation/src/test/resources/XpathTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\IdeaProjects\Cargo\CargoUIAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8E46ED-109E-42B4-8BF2-8C7AD4D67DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AB0DB2-9776-4117-A7F5-E1F7AD25CD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73F83708-58D9-CD41-B3DD-01428282C24F}"/>
   </bookViews>
@@ -705,24 +705,9 @@
     <t>input#gestationDestCode</t>
   </si>
   <si>
-    <t>input#gequantity-1</t>
-  </si>
-  <si>
     <t>input#gestationSourceCode</t>
   </si>
   <si>
-    <t>input#gelength-1</t>
-  </si>
-  <si>
-    <t>input#gewidth-1</t>
-  </si>
-  <si>
-    <t>input#geheight-1</t>
-  </si>
-  <si>
-    <t>select#geunit-1</t>
-  </si>
-  <si>
     <t>div#dc-tab-content156-6406 &gt; form &gt; div:nth-child(7) &gt; a</t>
   </si>
   <si>
@@ -1027,6 +1012,21 @@
   </si>
   <si>
     <t>//span[@id='awbNumber']</t>
+  </si>
+  <si>
+    <t>input#gequantity-%s</t>
+  </si>
+  <si>
+    <t>input#gelength-%s</t>
+  </si>
+  <si>
+    <t>input#gewidth-%s</t>
+  </si>
+  <si>
+    <t>input#geheight-%s</t>
+  </si>
+  <si>
+    <t>select#geunit-%s</t>
   </si>
 </sst>
 </file>
@@ -1422,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486E0D93-E580-4D4E-91BE-77049C6FF4F1}">
   <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A148" sqref="A148"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
@@ -2284,7 +2284,7 @@
         <v>203</v>
       </c>
       <c r="B106" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2297,50 +2297,50 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2348,7 +2348,7 @@
         <v>205</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2356,23 +2356,23 @@
         <v>206</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2388,7 +2388,7 @@
         <v>208</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>226</v>
+        <v>329</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2396,7 +2396,7 @@
         <v>209</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>228</v>
+        <v>330</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2404,7 +2404,7 @@
         <v>210</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>229</v>
+        <v>331</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2412,7 +2412,7 @@
         <v>211</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>230</v>
+        <v>332</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2420,7 +2420,7 @@
         <v>212</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>231</v>
+        <v>333</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2428,7 +2428,7 @@
         <v>213</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2436,7 +2436,7 @@
         <v>214</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2444,7 +2444,7 @@
         <v>215</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2452,7 +2452,7 @@
         <v>216</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2460,7 +2460,7 @@
         <v>217</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2468,7 +2468,7 @@
         <v>218</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2476,7 +2476,7 @@
         <v>219</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2484,7 +2484,7 @@
         <v>220</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2492,7 +2492,7 @@
         <v>221</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2500,7 +2500,7 @@
         <v>222</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2508,172 +2508,172 @@
         <v>223</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>53</v>
@@ -2681,154 +2681,154 @@
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>